<commit_message>
Checking in version 4.4.1, which removes binding options.
</commit_message>
<xml_diff>
--- a/Work Items/DataTier.Net 8 Planning.xlsx
+++ b/Work Items/DataTier.Net 8 Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GitHub\DataTier.Net\Work Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA8CE8CA-54E7-4887-8F19-5B5F0BA7FC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD29288-8173-4B3F-A180-45FA986571FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{79E08D5E-8E13-43AC-8E14-5BE41F2CFB46}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Title</t>
   </si>
@@ -54,10 +54,133 @@
     <t>When I first learned Blazor, I needed this. I don't think is needed now.</t>
   </si>
   <si>
-    <t>Easy - Just make sure the custom replacement code is gone also.</t>
-  </si>
-  <si>
     <t>Planning</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Make sure to update the User's Guide</t>
+  </si>
+  <si>
+    <t>Replace Stored Procedure Manager</t>
+  </si>
+  <si>
+    <t>Stored Procs were too object oriented. Replace with XML loaded.</t>
+  </si>
+  <si>
+    <t>Template Change Also</t>
+  </si>
+  <si>
+    <t>Remove App Logic Component</t>
+  </si>
+  <si>
+    <t>Move Connection to DAC</t>
+  </si>
+  <si>
+    <t>Major - Remove code generated stored procs and builders.</t>
+  </si>
+  <si>
+    <t>Medium - Move everything to DAC - Investigate removing Data Operations</t>
+  </si>
+  <si>
+    <t>Move Gateway to DAC</t>
+  </si>
+  <si>
+    <t>This gets it down to 2 projects</t>
+  </si>
+  <si>
+    <t>Medium - Code Generation and Custom Methods has to change</t>
+  </si>
+  <si>
+    <t>Move Object Library To DAC</t>
+  </si>
+  <si>
+    <t>This gets it down 1 project</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Visual Studio Project Updater</t>
+  </si>
+  <si>
+    <t>Redesign form and control for 1 project</t>
+  </si>
+  <si>
+    <t>Update Documentation</t>
+  </si>
+  <si>
+    <t>Lots of the Users Guide and Quick Start Will Change</t>
+  </si>
+  <si>
+    <t>New Install Release</t>
+  </si>
+  <si>
+    <t>Update the installer</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Benchmarks</t>
+  </si>
+  <si>
+    <t>Test if there are any performance gaines</t>
+  </si>
+  <si>
+    <t>Update Project Template</t>
+  </si>
+  <si>
+    <t>This goes from a multi-project template to single</t>
+  </si>
+  <si>
+    <t>Build Copy should handle this</t>
+  </si>
+  <si>
+    <t>Change Custom Method Editors</t>
+  </si>
+  <si>
+    <t>Use XML and make sure build rewrites base and custom methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Major </t>
+  </si>
+  <si>
+    <t>Remove Binding</t>
+  </si>
+  <si>
+    <t>Take out code for AllowBinding and Code Generation of ItemCallback</t>
+  </si>
+  <si>
+    <t>Medium - Took out the DataGateway code</t>
+  </si>
+  <si>
+    <t>Medium - Effects code generation and GUI</t>
+  </si>
+  <si>
+    <t>Required update to DataJuggler.Net (.NET Framework version)</t>
+  </si>
+  <si>
+    <t>Fix Indent for Custom Methods</t>
+  </si>
+  <si>
+    <t>VS 2022 indent doesn't like indented regions</t>
+  </si>
+  <si>
+    <t>Indent is 1 tab to indented.</t>
+  </si>
+  <si>
+    <t>Remove Order By Descending</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field Set </t>
+  </si>
+  <si>
+    <t>Done Except Docs &amp; Testing</t>
+  </si>
+  <si>
+    <t>Done Except Testing</t>
   </si>
 </sst>
 </file>
@@ -81,12 +204,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -101,9 +230,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,20 +548,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED85CC5-24CE-4191-A7D7-65F85A3C6293}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.19921875" customWidth="1"/>
+    <col min="1" max="1" width="28.69921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,19 +576,222 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>